<commit_message>
add 5 task (fish)
</commit_message>
<xml_diff>
--- a/Коммуникационный_план.xlsx
+++ b/Коммуникационный_план.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Заинтересованные стороны:</t>
   </si>
@@ -118,6 +118,66 @@
   </si>
   <si>
     <t xml:space="preserve">Дает предварительную оценку успешности продукта относительно конкурентов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Управление коммуникацией с каждой группой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Какая информация требуется участнику или группе?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кто будет её передавать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Как часто нужно её передавать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">По каким каналам связи её будут передавать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус выполнения проекта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">по Agile - каждые 2 недели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Личная встреча</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Какие ранне поставленные задачи выполнены</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Система учета (WEEEK.ru) и митинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раз в день для корректировки планов при возникновеннии проблем</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Онлайн и offline встречи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Описание проекта, цель проекта, реализованные функции, графические материалы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Через мессенджер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Списко задач с временем отведенным на их выполнение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раз в 2 недели, но необходима промежуточная корректировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Описание проекта, новые функции и преимущества</t>
+  </si>
+  <si>
+    <t>Макетолог</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раз в 2 недели, но можно чаще, при исправлении багов или оповешении пользователей о выгодных предложениях</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Социальные сети, реклама на других сайтах</t>
   </si>
 </sst>
 </file>
@@ -137,7 +197,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +214,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor theme="4" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.099978637043366805"/>
+        <bgColor theme="2" tint="-0.099978637043366805"/>
       </patternFill>
     </fill>
   </fills>
@@ -184,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +259,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -209,6 +281,13 @@
     </xf>
     <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,128 +820,238 @@
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="28.5">
       <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" ht="72" customHeight="1">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="99.75">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" ht="71.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" ht="85.5">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="10" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" ht="42.75">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" ht="42.75">
+      <c r="B15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" ht="57">
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" ht="42.75">
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" ht="57">
+      <c r="B18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>